<commit_message>
Reviewed Ivans user stories and added comments
</commit_message>
<xml_diff>
--- a/User Stories/Invoice&SubscriptionUserStories.xlsx
+++ b/User Stories/Invoice&SubscriptionUserStories.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ivanl\Documents\GitHub\Newsagent-Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Palej\Desktop\Software Design with AI for Cloud\Year_3\agile-labs3\Newsagent-Project\User Stories\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12F8C58C-265A-495E-BFDB-DD25BF11197C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{313D8D29-84E3-4D60-B1F4-F2BE243180A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="13120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,6 +22,68 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={50348294-397F-4282-9D4E-706A3713BFFD}</author>
+    <author>tc={316F6F9D-7187-4BE6-816B-E4EC67CD6985}</author>
+    <author>tc={7C66BF3C-6828-4EDA-8EC4-23D440AE43F5}</author>
+    <author>tc={BBC6AFCC-C181-4E2F-BC6F-2613B12B02D5}</author>
+    <author>tc={CC847E32-A7E8-490D-BEF1-C319BB838B37}</author>
+  </authors>
+  <commentList>
+    <comment ref="E6" authorId="0" shapeId="0" xr:uid="{50348294-397F-4282-9D4E-706A3713BFFD}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    I think we are missing here some details. We want to create subscription, but whats there, just subType? I think we need custDetails + publications cust is getting delivered. We need to verify details of books that cust will be getting or maybe say something like "verify publication can be added to subscruption"?</t>
+      </text>
+    </comment>
+    <comment ref="E8" authorId="1" shapeId="0" xr:uid="{316F6F9D-7187-4BE6-816B-E4EC67CD6985}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    I would also add cust name/last time for more clarity ☺️</t>
+      </text>
+    </comment>
+    <comment ref="E11" authorId="2" shapeId="0" xr:uid="{7C66BF3C-6828-4EDA-8EC4-23D440AE43F5}">
+      <text>
+        <t xml:space="preserve">[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    You will need to add acceptance criteria that verifies cust subscription details were successfully updated, eg
+Verify subscriptionType was updated 
+Verify publications were updated etc
+Reply:
+    Maybe also something like
+Verify publication can be deleted from sub
+Verify publication can be added to sub
+Verify delivery frequency can be updated </t>
+      </text>
+    </comment>
+    <comment ref="E16" authorId="3" shapeId="0" xr:uid="{BBC6AFCC-C181-4E2F-BC6F-2613B12B02D5}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    When we talk about subscription are we talking about the whole customer sub or just one particular book? 
+I think we also need to add something to veirfy the correct user is selected. How do we verify its been deleted for the right user? Maybe "verify prompt "enter user ID/userName/userLastName to manage subscriptions" ? Idk</t>
+      </text>
+    </comment>
+    <comment ref="E21" authorId="4" shapeId="0" xr:uid="{CC847E32-A7E8-490D-BEF1-C319BB838B37}">
+      <text>
+        <t xml:space="preserve">[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Same comment here as in the acceptance criteria 3. Is this read subscriptions in general for everyone or for specific customer? We should verify that correct cust is selected </t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -179,7 +241,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -224,6 +286,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="6">
@@ -348,44 +416,44 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -405,7 +473,9 @@
 </file>
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Natalia Palej" id="{188CBBDB-88B2-46D5-89F6-17778A888F38}" userId="cad1acabf18afac6" providerId="Windows Live"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -669,25 +739,54 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="E6" dT="2023-10-06T10:40:54.33" personId="{188CBBDB-88B2-46D5-89F6-17778A888F38}" id="{50348294-397F-4282-9D4E-706A3713BFFD}">
+    <text>I think we are missing here some details. We want to create subscription, but whats there, just subType? I think we need custDetails + publications cust is getting delivered. We need to verify details of books that cust will be getting or maybe say something like "verify publication can be added to subscruption"?</text>
+  </threadedComment>
+  <threadedComment ref="E8" dT="2023-10-06T10:37:12.10" personId="{188CBBDB-88B2-46D5-89F6-17778A888F38}" id="{316F6F9D-7187-4BE6-816B-E4EC67CD6985}">
+    <text>I would also add cust name/last time for more clarity ☺️</text>
+  </threadedComment>
+  <threadedComment ref="E11" dT="2023-10-06T10:38:50.11" personId="{188CBBDB-88B2-46D5-89F6-17778A888F38}" id="{7C66BF3C-6828-4EDA-8EC4-23D440AE43F5}">
+    <text>You will need to add acceptance criteria that verifies cust subscription details were successfully updated, eg
+Verify subscriptionType was updated 
+Verify publications were updated etc</text>
+  </threadedComment>
+  <threadedComment ref="E11" dT="2023-10-06T10:41:58.38" personId="{188CBBDB-88B2-46D5-89F6-17778A888F38}" id="{FA469C39-DD3A-4518-83A3-C6AC679D58C2}" parentId="{7C66BF3C-6828-4EDA-8EC4-23D440AE43F5}">
+    <text xml:space="preserve">Maybe also something like
+Verify publication can be deleted from sub
+Verify publication can be added to sub
+Verify delivery frequency can be updated </text>
+  </threadedComment>
+  <threadedComment ref="E16" dT="2023-10-06T10:43:34.37" personId="{188CBBDB-88B2-46D5-89F6-17778A888F38}" id="{BBC6AFCC-C181-4E2F-BC6F-2613B12B02D5}">
+    <text>When we talk about subscription are we talking about the whole customer sub or just one particular book? 
+I think we also need to add something to veirfy the correct user is selected. How do we verify its been deleted for the right user? Maybe "verify prompt "enter user ID/userName/userLastName to manage subscriptions" ? Idk</text>
+  </threadedComment>
+  <threadedComment ref="E21" dT="2023-10-06T10:44:21.22" personId="{188CBBDB-88B2-46D5-89F6-17778A888F38}" id="{CC847E32-A7E8-490D-BEF1-C319BB838B37}">
+    <text xml:space="preserve">Same comment here as in the acceptance criteria 3. Is this read subscriptions in general for everyone or for specific customer? We should verify that correct cust is selected </text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F36"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="2.81640625" customWidth="1"/>
-    <col min="2" max="2" width="13.08984375" customWidth="1"/>
-    <col min="3" max="3" width="31.7265625" customWidth="1"/>
+    <col min="1" max="1" width="2.796875" customWidth="1"/>
+    <col min="2" max="2" width="13.06640625" customWidth="1"/>
+    <col min="3" max="3" width="31.73046875" customWidth="1"/>
     <col min="4" max="4" width="38" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="81" style="7" customWidth="1"/>
-    <col min="6" max="6" width="63.7265625" customWidth="1"/>
+    <col min="6" max="6" width="63.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>17</v>
       </c>
@@ -707,420 +806,453 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="18">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A2" s="23">
         <v>1</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="22" t="s">
+      <c r="E2" s="14" t="s">
         <v>6</v>
       </c>
       <c r="F2" s="4"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="18"/>
-      <c r="B3" s="13"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="22" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A3" s="23"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="14" t="s">
         <v>23</v>
       </c>
       <c r="F3" s="4"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="18"/>
-      <c r="B4" s="13"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="19" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A4" s="23"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="12" t="s">
         <v>29</v>
       </c>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" s="18"/>
-      <c r="B5" s="13"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="22" t="s">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A5" s="23"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="14" t="s">
         <v>24</v>
       </c>
       <c r="F5" s="4"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" s="18"/>
-      <c r="B6" s="13"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="22" t="s">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A6" s="23"/>
+      <c r="B6" s="17"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="4"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A7" s="23"/>
+      <c r="B7" s="17"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="4"/>
-    </row>
-    <row r="7" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A7" s="18"/>
-      <c r="B7" s="15"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="15"/>
-      <c r="E7" s="19" t="s">
+      <c r="F7" s="4"/>
+    </row>
+    <row r="8" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A8" s="23"/>
+      <c r="B8" s="18"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="F7" s="4"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8" s="5"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A9" s="20">
+      <c r="F8" s="4"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A9" s="5"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A10" s="22">
         <v>2</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B10" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C10" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="11" t="s">
+      <c r="D10" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="23" t="s">
+      <c r="E10" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="F10" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A10" s="20"/>
-      <c r="B10" s="13"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="9" t="s">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A11" s="22"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="4"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A12" s="22"/>
+      <c r="B12" s="17"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="F10" s="4"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11" s="20"/>
-      <c r="B11" s="15"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="9" t="s">
+      <c r="F12" s="4"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A13" s="22"/>
+      <c r="B13" s="18"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="F11" s="4"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A12" s="5"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="21"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A13" s="20">
+      <c r="F13" s="4"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A14" s="5"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="13"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A15" s="22">
         <v>3</v>
       </c>
-      <c r="B13" s="11" t="s">
+      <c r="B15" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C15" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="D13" s="11" t="s">
+      <c r="D15" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="E13" s="9" t="s">
+      <c r="E15" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="F13" s="4" t="s">
+      <c r="F15" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A14" s="20"/>
-      <c r="B14" s="13"/>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="F14" s="4"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A15" s="20"/>
-      <c r="B15" s="15"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="F15" s="4"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A16" s="5"/>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A16" s="22"/>
       <c r="B16" s="17"/>
       <c r="C16" s="17"/>
       <c r="D16" s="17"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="21"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A17" s="20">
+      <c r="E16" s="9"/>
+      <c r="F16" s="4"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A17" s="22"/>
+      <c r="B17" s="17"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="F17" s="4"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A18" s="22"/>
+      <c r="B18" s="18"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F18" s="4"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A19" s="5"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="13"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A20" s="22">
         <v>4</v>
       </c>
-      <c r="B17" s="11" t="s">
+      <c r="B20" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="C17" s="11" t="s">
+      <c r="C20" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="D17" s="11" t="s">
+      <c r="D20" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="E17" s="9" t="s">
+      <c r="E20" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="F17" s="4"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A18" s="20"/>
-      <c r="B18" s="15"/>
-      <c r="C18" s="15"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="9" t="s">
+      <c r="F20" s="4"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A21" s="22"/>
+      <c r="B21" s="17"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="4"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A22" s="22"/>
+      <c r="B22" s="18"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="F18" s="4"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A19" s="5"/>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="21"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B20" s="11" t="s">
+      <c r="F22" s="4"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A23" s="5"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="13"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="B24" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="C20" s="12" t="s">
+      <c r="C24" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="D20" s="11" t="s">
+      <c r="D24" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="E20" s="19" t="s">
+      <c r="E24" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="F20" s="4"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B21" s="13"/>
-      <c r="C21" s="14"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="19" t="s">
+      <c r="F24" s="4"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="B25" s="17"/>
+      <c r="C25" s="20"/>
+      <c r="D25" s="17"/>
+      <c r="E25" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="F21" s="4"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B22" s="13"/>
-      <c r="C22" s="14"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="19" t="s">
+      <c r="F25" s="4"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="B26" s="17"/>
+      <c r="C26" s="20"/>
+      <c r="D26" s="17"/>
+      <c r="E26" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="F22" s="4"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B23" s="13"/>
-      <c r="C23" s="14"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="19" t="s">
+      <c r="F26" s="4"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="B27" s="17"/>
+      <c r="C27" s="20"/>
+      <c r="D27" s="17"/>
+      <c r="E27" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="F23" s="4"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B24" s="13"/>
-      <c r="C24" s="14"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="19" t="s">
+      <c r="F27" s="4"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="B28" s="17"/>
+      <c r="C28" s="20"/>
+      <c r="D28" s="17"/>
+      <c r="E28" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="F24" s="4"/>
-    </row>
-    <row r="25" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="B25" s="15"/>
-      <c r="C25" s="16"/>
-      <c r="D25" s="15"/>
-      <c r="E25" s="19" t="s">
+      <c r="F28" s="4"/>
+    </row>
+    <row r="29" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B29" s="18"/>
+      <c r="C29" s="21"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="F25" s="4"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="10"/>
-      <c r="E26" s="8"/>
-      <c r="F26" s="8"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B27" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="C27" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="D27" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="E27" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="F27" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B28" s="13"/>
-      <c r="C28" s="13"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="F28" s="4"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B29" s="15"/>
-      <c r="C29" s="15"/>
-      <c r="D29" s="15"/>
-      <c r="E29" s="9" t="s">
-        <v>11</v>
-      </c>
       <c r="F29" s="4"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B30" s="6"/>
       <c r="C30" s="6"/>
-      <c r="D30" s="6"/>
+      <c r="D30" s="10"/>
       <c r="E30" s="8"/>
-      <c r="F30" s="21"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B31" s="11" t="s">
+      <c r="F30" s="8"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="B31" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="C31" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="D31" s="11" t="s">
-        <v>12</v>
+      <c r="C31" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="D31" s="16" t="s">
+        <v>9</v>
       </c>
       <c r="E31" s="9" t="s">
         <v>6</v>
       </c>
       <c r="F31" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="B32" s="17"/>
+      <c r="C32" s="17"/>
+      <c r="D32" s="17"/>
+      <c r="E32" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F32" s="4"/>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B33" s="18"/>
+      <c r="C33" s="18"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F33" s="4"/>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B34" s="6"/>
+      <c r="C34" s="6"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="8"/>
+      <c r="F34" s="13"/>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B35" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C35" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="D35" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="E35" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="F35" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B32" s="13"/>
-      <c r="C32" s="13"/>
-      <c r="D32" s="13"/>
-      <c r="E32" s="9" t="s">
+    <row r="36" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B36" s="17"/>
+      <c r="C36" s="17"/>
+      <c r="D36" s="17"/>
+      <c r="E36" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="F32" s="4"/>
-    </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B33" s="15"/>
-      <c r="C33" s="15"/>
-      <c r="D33" s="15"/>
-      <c r="E33" s="9" t="s">
+      <c r="F36" s="4"/>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B37" s="18"/>
+      <c r="C37" s="18"/>
+      <c r="D37" s="18"/>
+      <c r="E37" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="F33" s="4"/>
-    </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B34" s="17"/>
-      <c r="C34" s="17"/>
-      <c r="D34" s="17"/>
-      <c r="E34" s="8"/>
-      <c r="F34" s="21"/>
-    </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B35" s="11" t="s">
+      <c r="F37" s="4"/>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B38" s="11"/>
+      <c r="C38" s="11"/>
+      <c r="D38" s="11"/>
+      <c r="E38" s="8"/>
+      <c r="F38" s="13"/>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B39" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="C35" s="11" t="s">
+      <c r="C39" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="D35" s="11" t="s">
+      <c r="D39" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="E35" s="9" t="s">
+      <c r="E39" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="F35" s="4"/>
-    </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B36" s="15"/>
-      <c r="C36" s="15"/>
-      <c r="D36" s="15"/>
-      <c r="E36" s="9" t="s">
+      <c r="F39" s="4"/>
+    </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B40" s="18"/>
+      <c r="C40" s="18"/>
+      <c r="D40" s="18"/>
+      <c r="E40" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="F36" s="4"/>
+      <c r="F40" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="D31:D33"/>
-    <mergeCell ref="B35:B36"/>
-    <mergeCell ref="C35:C36"/>
-    <mergeCell ref="D35:D36"/>
-    <mergeCell ref="B20:B25"/>
-    <mergeCell ref="C20:C25"/>
-    <mergeCell ref="D20:D25"/>
-    <mergeCell ref="B27:B29"/>
-    <mergeCell ref="C27:C29"/>
-    <mergeCell ref="D27:D29"/>
+    <mergeCell ref="A2:A8"/>
+    <mergeCell ref="B2:B8"/>
+    <mergeCell ref="C2:C8"/>
+    <mergeCell ref="D2:D8"/>
+    <mergeCell ref="A20:A22"/>
+    <mergeCell ref="B20:B22"/>
+    <mergeCell ref="C20:C22"/>
+    <mergeCell ref="D20:D22"/>
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="B10:B13"/>
+    <mergeCell ref="C10:C13"/>
+    <mergeCell ref="D10:D13"/>
+    <mergeCell ref="A15:A18"/>
+    <mergeCell ref="B15:B18"/>
+    <mergeCell ref="C15:C18"/>
+    <mergeCell ref="D15:D18"/>
+    <mergeCell ref="D35:D37"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="C39:C40"/>
+    <mergeCell ref="D39:D40"/>
+    <mergeCell ref="B24:B29"/>
+    <mergeCell ref="C24:C29"/>
+    <mergeCell ref="D24:D29"/>
     <mergeCell ref="B31:B33"/>
     <mergeCell ref="C31:C33"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="A9:A11"/>
-    <mergeCell ref="B9:B11"/>
-    <mergeCell ref="C9:C11"/>
-    <mergeCell ref="D9:D11"/>
-    <mergeCell ref="A13:A15"/>
-    <mergeCell ref="B13:B15"/>
-    <mergeCell ref="C13:C15"/>
-    <mergeCell ref="D13:D15"/>
-    <mergeCell ref="A2:A7"/>
-    <mergeCell ref="B2:B7"/>
-    <mergeCell ref="C2:C7"/>
-    <mergeCell ref="D2:D7"/>
+    <mergeCell ref="D31:D33"/>
+    <mergeCell ref="B35:B37"/>
+    <mergeCell ref="C35:C37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Reviewed Ivan's User Stories and added comments
</commit_message>
<xml_diff>
--- a/User Stories/Invoice&SubscriptionUserStories.xlsx
+++ b/User Stories/Invoice&SubscriptionUserStories.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ivan\Desktop\Github\Newsagent-Project\User Stories\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Palej\Desktop\Software Design with AI for Cloud\Year_3\agile-labs3\Newsagent-Project\User Stories\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D57FEAB-4C08-44AB-8C9C-CD7488568464}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0CF0192-B353-4F82-B45D-ED1957BAA57F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,44 +27,53 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>tc={50348294-397F-4282-9D4E-706A3713BFFD}</author>
-    <author>tc={316F6F9D-7187-4BE6-816B-E4EC67CD6985}</author>
-    <author>tc={7C66BF3C-6828-4EDA-8EC4-23D440AE43F5}</author>
+    <author>tc={E8DB2F73-A78D-4E88-B0B4-BAF1D56B9ABE}</author>
+    <author>tc={B592C4EC-EA24-4D3F-B3F5-666E5FD068EA}</author>
+    <author>tc={98E88FF4-C514-459A-A18F-20335A6A4D76}</author>
+    <author>tc={B7E2F2D2-72A4-4CDE-BD3E-530DB675E87B}</author>
+    <author>tc={18B85A84-1733-4947-9750-AFC5955B39C3}</author>
   </authors>
   <commentList>
-    <comment ref="E8" authorId="0" shapeId="0" xr:uid="{50348294-397F-4282-9D4E-706A3713BFFD}">
+    <comment ref="E18" authorId="0" shapeId="0" xr:uid="{E8DB2F73-A78D-4E88-B0B4-BAF1D56B9ABE}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
-    I think we are missing here some details. We want to create subscription, but whats there, just subType? I think we need custDetails + publications cust is getting delivered. We need to verify details of books that cust will be getting or maybe say something like "verify publication can be added to subscruption"?
+    Not needed, we shouldn’t be changing date of sub at all, it should be by default first day that cust signed in for specific book
 Reply:
-    Very good question Natalia .  I'm going to include some from your Database Tables as in Team Plan Document. </t>
+    Or is it more as a precaution in case if date is wrong? </t>
       </text>
     </comment>
-    <comment ref="E11" authorId="1" shapeId="0" xr:uid="{316F6F9D-7187-4BE6-816B-E4EC67CD6985}">
+    <comment ref="E48" authorId="1" shapeId="0" xr:uid="{B592C4EC-EA24-4D3F-B3F5-666E5FD068EA}">
       <text>
-        <t xml:space="preserve">[Threaded comment]
+        <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
-    I would also add cust name/last time for more clarity ☺️
-Reply:
-    👌 </t>
+    I don’t think its needed, we only should be updating invoice details, why mention subscription?</t>
       </text>
     </comment>
-    <comment ref="E14" authorId="2" shapeId="0" xr:uid="{7C66BF3C-6828-4EDA-8EC4-23D440AE43F5}">
+    <comment ref="E49" authorId="2" shapeId="0" xr:uid="{98E88FF4-C514-459A-A18F-20335A6A4D76}">
       <text>
-        <t xml:space="preserve">[Threaded comment]
+        <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
-    You will need to add acceptance criteria that verifies cust subscription details were successfully updated, eg
-Verify subscriptionType was updated 
-Verify publications were updated etc
-Reply:
-    Maybe also something like
-Verify publication can be deleted from sub
-Verify publication can be added to sub
-Verify delivery frequency can be updated </t>
+    I don’t think its needed</t>
+      </text>
+    </comment>
+    <comment ref="E50" authorId="3" shapeId="0" xr:uid="{B7E2F2D2-72A4-4CDE-BD3E-530DB675E87B}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Not needed, the date of invoice shouldn’t change</t>
+      </text>
+    </comment>
+    <comment ref="E51" authorId="4" shapeId="0" xr:uid="{18B85A84-1733-4947-9750-AFC5955B39C3}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    I don’t think its needed</t>
       </text>
     </comment>
   </commentList>
@@ -72,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="69">
   <si>
     <t>WHO</t>
   </si>
@@ -92,9 +101,6 @@
     <t>As an admin</t>
   </si>
   <si>
-    <t>Verify admin is successfully logged in</t>
-  </si>
-  <si>
     <t xml:space="preserve">Verify errors are handled properly </t>
   </si>
   <si>
@@ -131,9 +137,6 @@
     <t>Verify subscription doesn't already exist in database</t>
   </si>
   <si>
-    <t>Verifiy message "subsciption successfully deleted" is displayed</t>
-  </si>
-  <si>
     <t>Verifiy subscription was deleted succesfully</t>
   </si>
   <si>
@@ -155,9 +158,6 @@
     <t>Verify subscription details have been updated successfully</t>
   </si>
   <si>
-    <t xml:space="preserve">Verify message "subscription successfully updated + subscriptionDetails() " is displayed </t>
-  </si>
-  <si>
     <t>Verify valid subscriptionType == daily || weekly || monthly assigned to subscription</t>
   </si>
   <si>
@@ -182,9 +182,6 @@
     <t>Use searchSubscription() to verify account was deleted</t>
   </si>
   <si>
-    <t>Use printSubscriptionDetails() to verify details were updated</t>
-  </si>
-  <si>
     <t>Verify subscription assigned to different customer.</t>
   </si>
   <si>
@@ -194,18 +191,12 @@
     <t>Verify subscription startDate changed succesfully</t>
   </si>
   <si>
-    <t>Verify publication name was updated succesfully</t>
-  </si>
-  <si>
     <t>so that I can remove subscriptions customert no longer desires.</t>
   </si>
   <si>
     <t>so that I can view subscription details</t>
   </si>
   <si>
-    <t>Use searchSubscription() to verify Subscription was deleted</t>
-  </si>
-  <si>
     <t>Verify SubscriptionDetails read succesfully</t>
   </si>
   <si>
@@ -224,15 +215,9 @@
     <t>Verify message "invoice " + invoiceID, customerID ,  subscriptionID + "succesfully created"</t>
   </si>
   <si>
-    <t>Verify  invoice customer is changed succesfully</t>
-  </si>
-  <si>
     <t>Verify invoice subscription is changed  succesfully</t>
   </si>
   <si>
-    <t>Verify  message "invoice customer" +invoiceID, CustomerID+"is changed succesfully"</t>
-  </si>
-  <si>
     <t>Verify  message "invoice subscription" +invoiceID, subscriptionID+"is changed succesfully"</t>
   </si>
   <si>
@@ -242,32 +227,284 @@
     <t>Verify  message "invoice date" +invoiceID, invoiceDate+"is changed succesfully"</t>
   </si>
   <si>
-    <t>Verify that invoice appeared after search.</t>
-  </si>
-  <si>
-    <t>Verify that subscription appeared after search.</t>
-  </si>
-  <si>
-    <t>Verify invoice deleted succesfully</t>
-  </si>
-  <si>
     <t>Verify message "invoice"+ InvoiceID+ "deleted succesfully"</t>
   </si>
   <si>
     <t>Verify message "invoice"+ InvoiceID+ "not found"</t>
   </si>
   <si>
-    <t>Verify that invoice did not  appeared after search.</t>
-  </si>
-  <si>
     <t>Verify invoiceDetails read succesfully</t>
+  </si>
+  <si>
+    <t>Verify newsagent is successfully logged in</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This is to capture WHEN someone signed up just so we know the start date </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Verify that subscription appeared after search </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>for a specific customer</t>
+    </r>
+  </si>
+  <si>
+    <t>Not sure what you mean?</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Verify publication </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>title</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> was updated succesfully</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Verify message "subscription successfully updated + subscriptionDetails() </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">+ customerFullName </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">" is displayed  </t>
+    </r>
+  </si>
+  <si>
+    <t>Verify newsagent succesfully loged out</t>
+  </si>
+  <si>
+    <t>Verify message "are you sure you want to delete subscription &lt;subscriptionID&gt; for custFullName" YES/NO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify if "NO" nothing happens </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Verifiy </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">if "YES" </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>message "subsciption successfully deleted" is displayed</t>
+    </r>
+  </si>
+  <si>
+    <t>Use subscriptionDetails() to verify details were updated</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As Im reading this, am I wrong thinking the invoice should be automatically created since we will fetch ALL the details (custDetails + publications + subscription)? Do we actually want to create them? Or maybe lets add this in case if it isnt automatically created </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Verify that invoice appeared after search </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>for a specific customer</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Verify customer invoice is </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>updated</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> succesfully</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Verify message "Invoice " + invoiceID, CustomerID + "</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>was updated</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> succesfully"</t>
+    </r>
+  </si>
+  <si>
+    <t>Verify message appears "are you sure you want to delete Invoice invoiceID for custFullName?" YES/NO</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Verify </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>if "YES"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> invoice deleted succesfully</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Verify that </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>invalid</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> invoice </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ID</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> did not appeared after search</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -312,8 +549,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -332,8 +590,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -356,11 +626,42 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -393,35 +694,60 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -441,7 +767,6 @@
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <person displayName="Ivan Lapickij" id="{D7BC6C5A-621E-4C0A-9CC2-52B042B0A4F3}" userId="86cab317083f9d19" providerId="Windows Live"/>
   <person displayName="Natalia Palej" id="{188CBBDB-88B2-46D5-89F6-17778A888F38}" userId="cad1acabf18afac6" providerId="Windows Live"/>
 </personList>
 </file>
@@ -709,53 +1034,48 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="E8" dT="2023-10-06T10:40:54.33" personId="{188CBBDB-88B2-46D5-89F6-17778A888F38}" id="{50348294-397F-4282-9D4E-706A3713BFFD}" done="1">
-    <text>I think we are missing here some details. We want to create subscription, but whats there, just subType? I think we need custDetails + publications cust is getting delivered. We need to verify details of books that cust will be getting or maybe say something like "verify publication can be added to subscruption"?</text>
+  <threadedComment ref="E18" dT="2023-10-09T10:18:44.32" personId="{188CBBDB-88B2-46D5-89F6-17778A888F38}" id="{E8DB2F73-A78D-4E88-B0B4-BAF1D56B9ABE}">
+    <text>Not needed, we shouldn’t be changing date of sub at all, it should be by default first day that cust signed in for specific book</text>
   </threadedComment>
-  <threadedComment ref="E8" dT="2023-10-07T13:21:54.76" personId="{D7BC6C5A-621E-4C0A-9CC2-52B042B0A4F3}" id="{63F1D8C0-31E8-4075-8578-FC634E7FD05A}" parentId="{50348294-397F-4282-9D4E-706A3713BFFD}">
-    <text xml:space="preserve">Very good question Natalia .  I'm going to include some from your Database Tables as in Team Plan Document. </text>
+  <threadedComment ref="E18" dT="2023-10-09T10:19:03.25" personId="{188CBBDB-88B2-46D5-89F6-17778A888F38}" id="{AB796589-9E1A-4CA1-995E-13F400892EEA}" parentId="{E8DB2F73-A78D-4E88-B0B4-BAF1D56B9ABE}">
+    <text xml:space="preserve">Or is it more as a precaution in case if date is wrong? </text>
   </threadedComment>
-  <threadedComment ref="E11" dT="2023-10-06T10:37:12.10" personId="{188CBBDB-88B2-46D5-89F6-17778A888F38}" id="{316F6F9D-7187-4BE6-816B-E4EC67CD6985}" done="1">
-    <text>I would also add cust name/last time for more clarity ☺️</text>
+  <threadedComment ref="E48" dT="2023-10-09T10:18:03.06" personId="{188CBBDB-88B2-46D5-89F6-17778A888F38}" id="{B592C4EC-EA24-4D3F-B3F5-666E5FD068EA}">
+    <text>I don’t think its needed, we only should be updating invoice details, why mention subscription?</text>
   </threadedComment>
-  <threadedComment ref="E11" dT="2023-10-07T14:20:24.07" personId="{D7BC6C5A-621E-4C0A-9CC2-52B042B0A4F3}" id="{8FB90777-201A-4B4F-9AC0-05E2E9B320D9}" parentId="{316F6F9D-7187-4BE6-816B-E4EC67CD6985}">
-    <text xml:space="preserve">👌 </text>
+  <threadedComment ref="E49" dT="2023-10-09T10:17:42.97" personId="{188CBBDB-88B2-46D5-89F6-17778A888F38}" id="{98E88FF4-C514-459A-A18F-20335A6A4D76}">
+    <text>I don’t think its needed</text>
   </threadedComment>
-  <threadedComment ref="E14" dT="2023-10-06T10:38:50.11" personId="{188CBBDB-88B2-46D5-89F6-17778A888F38}" id="{7C66BF3C-6828-4EDA-8EC4-23D440AE43F5}">
-    <text>You will need to add acceptance criteria that verifies cust subscription details were successfully updated, eg
-Verify subscriptionType was updated 
-Verify publications were updated etc</text>
+  <threadedComment ref="E50" dT="2023-10-09T10:17:20.55" personId="{188CBBDB-88B2-46D5-89F6-17778A888F38}" id="{B7E2F2D2-72A4-4CDE-BD3E-530DB675E87B}">
+    <text>Not needed, the date of invoice shouldn’t change</text>
   </threadedComment>
-  <threadedComment ref="E14" dT="2023-10-06T10:41:58.38" personId="{188CBBDB-88B2-46D5-89F6-17778A888F38}" id="{FA469C39-DD3A-4518-83A3-C6AC679D58C2}" parentId="{7C66BF3C-6828-4EDA-8EC4-23D440AE43F5}">
-    <text xml:space="preserve">Maybe also something like
-Verify publication can be deleted from sub
-Verify publication can be added to sub
-Verify delivery frequency can be updated </text>
+  <threadedComment ref="E51" dT="2023-10-09T10:17:08.36" personId="{188CBBDB-88B2-46D5-89F6-17778A888F38}" id="{18B85A84-1733-4947-9750-AFC5955B39C3}">
+    <text>I don’t think its needed</text>
   </threadedComment>
 </ThreadedComments>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F64"/>
+  <dimension ref="A1:F68"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView tabSelected="1" topLeftCell="D42" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E65" sqref="E65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="2.85546875" customWidth="1"/>
+    <col min="1" max="1" width="2.86328125" customWidth="1"/>
     <col min="2" max="2" width="13" customWidth="1"/>
-    <col min="3" max="3" width="31.7109375" customWidth="1"/>
+    <col min="3" max="3" width="31.73046875" customWidth="1"/>
     <col min="4" max="4" width="38" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="81" style="7" customWidth="1"/>
-    <col min="6" max="6" width="63.7109375" customWidth="1"/>
+    <col min="6" max="6" width="63.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -773,115 +1093,117 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="13">
+    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A2" s="18">
         <v>1</v>
       </c>
       <c r="B2" s="19" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="F2" s="4"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="13"/>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A3" s="18"/>
       <c r="B3" s="19"/>
       <c r="C3" s="20"/>
       <c r="D3" s="19"/>
       <c r="E3" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F3" s="4"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="13"/>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A4" s="18"/>
       <c r="B4" s="19"/>
       <c r="C4" s="20"/>
       <c r="D4" s="19"/>
       <c r="E4" s="11" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="13"/>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A5" s="18"/>
       <c r="B5" s="19"/>
       <c r="C5" s="20"/>
       <c r="D5" s="19"/>
       <c r="E5" s="11" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F5" s="4"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="13"/>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A6" s="18"/>
       <c r="B6" s="19"/>
       <c r="C6" s="20"/>
       <c r="D6" s="19"/>
       <c r="E6" s="11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="13"/>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A7" s="18"/>
       <c r="B7" s="19"/>
       <c r="C7" s="20"/>
       <c r="D7" s="19"/>
-      <c r="E7" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="F7" s="4"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="13"/>
+      <c r="E7" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A8" s="18"/>
       <c r="B8" s="19"/>
       <c r="C8" s="20"/>
       <c r="D8" s="19"/>
       <c r="E8" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="13"/>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A9" s="18"/>
       <c r="B9" s="19"/>
       <c r="C9" s="20"/>
       <c r="D9" s="19"/>
       <c r="E9" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F9" s="4"/>
     </row>
-    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="13"/>
+    <row r="10" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A10" s="18"/>
       <c r="B10" s="19"/>
       <c r="C10" s="20"/>
       <c r="D10" s="19"/>
       <c r="E10" s="11" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="13"/>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A11" s="18"/>
       <c r="B11" s="19"/>
       <c r="C11" s="20"/>
       <c r="D11" s="19"/>
-      <c r="E11" s="11" t="s">
-        <v>32</v>
+      <c r="E11" s="15" t="s">
+        <v>57</v>
       </c>
       <c r="F11" s="4"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12" s="5"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
@@ -889,109 +1211,109 @@
       <c r="E12" s="8"/>
       <c r="F12" s="8"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="13">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A13" s="18">
         <v>2</v>
       </c>
       <c r="B13" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="D13" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="E13" s="16" t="s">
-        <v>6</v>
+      <c r="E13" s="14" t="s">
+        <v>51</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="13"/>
+        <v>61</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A14" s="18"/>
       <c r="B14" s="19"/>
       <c r="C14" s="19"/>
       <c r="D14" s="19"/>
-      <c r="E14" s="16" t="s">
-        <v>57</v>
+      <c r="E14" s="14" t="s">
+        <v>53</v>
       </c>
       <c r="F14" s="4"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="13"/>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A15" s="18"/>
       <c r="B15" s="19"/>
       <c r="C15" s="19"/>
       <c r="D15" s="19"/>
-      <c r="E15" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="F15" s="4"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="13"/>
+      <c r="E15" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="F15" s="23" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A16" s="18"/>
       <c r="B16" s="19"/>
       <c r="C16" s="19"/>
       <c r="D16" s="19"/>
-      <c r="E16" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="F16" s="14"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="13"/>
+      <c r="E16" s="33" t="s">
+        <v>55</v>
+      </c>
+      <c r="F16" s="13"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A17" s="18"/>
       <c r="B17" s="19"/>
       <c r="C17" s="19"/>
       <c r="D17" s="19"/>
-      <c r="E17" s="16" t="s">
-        <v>38</v>
+      <c r="E17" s="14" t="s">
+        <v>34</v>
       </c>
       <c r="F17" s="12"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="13"/>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A18" s="18"/>
       <c r="B18" s="19"/>
       <c r="C18" s="19"/>
       <c r="D18" s="19"/>
-      <c r="E18" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="F18" s="4" t="s">
+      <c r="E18" s="29" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="13"/>
+      <c r="F18" s="32"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A19" s="18"/>
       <c r="B19" s="19"/>
       <c r="C19" s="19"/>
       <c r="D19" s="19"/>
-      <c r="E19" s="16" t="s">
-        <v>26</v>
+      <c r="E19" s="14" t="s">
+        <v>24</v>
       </c>
       <c r="F19" s="4"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="13"/>
+    <row r="20" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A20" s="18"/>
       <c r="B20" s="19"/>
       <c r="C20" s="19"/>
       <c r="D20" s="19"/>
-      <c r="E20" s="16" t="s">
-        <v>27</v>
+      <c r="E20" s="14" t="s">
+        <v>56</v>
       </c>
       <c r="F20" s="4"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="13"/>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A21" s="18"/>
       <c r="B21" s="19"/>
       <c r="C21" s="19"/>
       <c r="D21" s="19"/>
-      <c r="E21" s="17" t="s">
-        <v>32</v>
+      <c r="E21" s="15" t="s">
+        <v>57</v>
       </c>
       <c r="F21" s="4"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A22" s="5"/>
       <c r="B22" s="6"/>
       <c r="C22" s="6"/>
@@ -999,489 +1321,532 @@
       <c r="E22" s="8"/>
       <c r="F22" s="8"/>
     </row>
-    <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="13">
+    <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A23" s="18">
         <v>3</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C23" s="19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D23" s="19" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="E23" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="F23" s="4"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="13"/>
+        <v>51</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A24" s="18"/>
       <c r="B24" s="19"/>
       <c r="C24" s="19"/>
       <c r="D24" s="19"/>
-      <c r="E24" s="16" t="s">
-        <v>57</v>
+      <c r="E24" s="14" t="s">
+        <v>53</v>
       </c>
       <c r="F24" s="4"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="13"/>
+    <row r="25" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A25" s="18"/>
       <c r="B25" s="19"/>
       <c r="C25" s="19"/>
       <c r="D25" s="19"/>
-      <c r="E25" s="11" t="s">
-        <v>20</v>
+      <c r="E25" s="24" t="s">
+        <v>58</v>
       </c>
       <c r="F25" s="4"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="13"/>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A26" s="18"/>
       <c r="B26" s="19"/>
       <c r="C26" s="19"/>
       <c r="D26" s="19"/>
-      <c r="E26" s="11" t="s">
-        <v>19</v>
+      <c r="E26" s="24" t="s">
+        <v>59</v>
       </c>
       <c r="F26" s="4"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="13"/>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A27" s="18"/>
       <c r="B27" s="19"/>
       <c r="C27" s="19"/>
       <c r="D27" s="19"/>
-      <c r="E27" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="F27" s="4"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="5"/>
-      <c r="B28" s="10"/>
-      <c r="C28" s="10"/>
-      <c r="D28" s="10"/>
-      <c r="E28" s="8"/>
-      <c r="F28" s="8"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="13">
+      <c r="E27" s="11" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A28" s="18"/>
+      <c r="B28" s="19"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="F28" s="4"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A29" s="18"/>
+      <c r="B29" s="19"/>
+      <c r="C29" s="19"/>
+      <c r="D29" s="19"/>
+      <c r="E29" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="F29" s="4"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A30" s="5"/>
+      <c r="B30" s="10"/>
+      <c r="C30" s="10"/>
+      <c r="D30" s="10"/>
+      <c r="E30" s="8"/>
+      <c r="F30" s="8"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A31" s="18">
         <v>4</v>
       </c>
-      <c r="B29" s="19" t="s">
+      <c r="B31" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C29" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="D29" s="19" t="s">
-        <v>42</v>
-      </c>
-      <c r="E29" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="F29" s="4"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="13"/>
-      <c r="B30" s="19"/>
-      <c r="C30" s="19"/>
-      <c r="D30" s="19"/>
-      <c r="E30" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="F30" s="4"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="13"/>
-      <c r="B31" s="19"/>
-      <c r="C31" s="19"/>
-      <c r="D31" s="19"/>
-      <c r="E31" s="22" t="s">
-        <v>44</v>
+      <c r="C31" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="D31" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="E31" s="11" t="s">
+        <v>51</v>
       </c>
       <c r="F31" s="4"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="13"/>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A32" s="18"/>
       <c r="B32" s="19"/>
       <c r="C32" s="19"/>
       <c r="D32" s="19"/>
-      <c r="E32" s="21" t="s">
-        <v>32</v>
+      <c r="E32" s="14" t="s">
+        <v>53</v>
       </c>
       <c r="F32" s="4"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="5"/>
-      <c r="B33" s="6"/>
-      <c r="C33" s="6"/>
-      <c r="D33" s="6"/>
-      <c r="E33" s="8"/>
-      <c r="F33" s="8"/>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="15">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A33" s="18"/>
+      <c r="B33" s="19"/>
+      <c r="C33" s="19"/>
+      <c r="D33" s="19"/>
+      <c r="E33" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="F33" s="4"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A34" s="18"/>
+      <c r="B34" s="19"/>
+      <c r="C34" s="19"/>
+      <c r="D34" s="19"/>
+      <c r="E34" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="F34" s="4"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A35" s="5"/>
+      <c r="B35" s="6"/>
+      <c r="C35" s="6"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="8"/>
+      <c r="F35" s="8"/>
+    </row>
+    <row r="36" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A36" s="21">
         <v>5</v>
       </c>
-      <c r="B34" s="19" t="s">
+      <c r="B36" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C34" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="D34" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="E34" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="F34" s="4"/>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="15"/>
-      <c r="B35" s="19"/>
-      <c r="C35" s="20"/>
-      <c r="D35" s="19"/>
-      <c r="E35" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="F35" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="15"/>
-      <c r="B36" s="19"/>
-      <c r="C36" s="20"/>
-      <c r="D36" s="19"/>
+      <c r="C36" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="D36" s="19" t="s">
+        <v>20</v>
+      </c>
       <c r="E36" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="F36" s="4"/>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="15"/>
+        <v>51</v>
+      </c>
+      <c r="F36" s="25" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A37" s="21"/>
       <c r="B37" s="19"/>
       <c r="C37" s="20"/>
       <c r="D37" s="19"/>
       <c r="E37" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="F37" s="4"/>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="15"/>
+        <v>39</v>
+      </c>
+      <c r="F37" s="26"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A38" s="21"/>
       <c r="B38" s="19"/>
       <c r="C38" s="20"/>
       <c r="D38" s="19"/>
-      <c r="E38" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="F38" s="4"/>
-    </row>
-    <row r="39" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="15"/>
+      <c r="E38" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="F38" s="26"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A39" s="21"/>
       <c r="B39" s="19"/>
       <c r="C39" s="20"/>
       <c r="D39" s="19"/>
       <c r="E39" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="F39" s="15"/>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="15"/>
+        <v>41</v>
+      </c>
+      <c r="F39" s="26"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A40" s="21"/>
       <c r="B40" s="19"/>
       <c r="C40" s="20"/>
       <c r="D40" s="19"/>
-      <c r="E40" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="F40" s="15"/>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="6"/>
-      <c r="B41" s="6"/>
-      <c r="C41" s="6"/>
-      <c r="D41" s="9"/>
-      <c r="E41" s="8"/>
-      <c r="F41" s="8"/>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="15">
+      <c r="E40" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="F40" s="27"/>
+    </row>
+    <row r="41" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A41" s="21"/>
+      <c r="B41" s="19"/>
+      <c r="C41" s="20"/>
+      <c r="D41" s="19"/>
+      <c r="E41" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="F41" s="27"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A42" s="21"/>
+      <c r="B42" s="19"/>
+      <c r="C42" s="20"/>
+      <c r="D42" s="19"/>
+      <c r="E42" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="F42" s="28"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A43" s="6"/>
+      <c r="B43" s="6"/>
+      <c r="C43" s="6"/>
+      <c r="D43" s="9"/>
+      <c r="E43" s="8"/>
+      <c r="F43" s="8"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A44" s="21">
         <v>6</v>
       </c>
-      <c r="B42" s="19" t="s">
+      <c r="B44" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="C44" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="D44" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="C42" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="D42" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="E42" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="F42" s="4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="15"/>
-      <c r="B43" s="19"/>
-      <c r="C43" s="19"/>
-      <c r="D43" s="19"/>
-      <c r="E43" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="F43" s="4"/>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="15"/>
-      <c r="B44" s="19"/>
-      <c r="C44" s="19"/>
-      <c r="D44" s="19"/>
-      <c r="E44" s="16" t="s">
-        <v>50</v>
+      <c r="E44" s="11" t="s">
+        <v>51</v>
       </c>
       <c r="F44" s="4"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="15"/>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A45" s="21"/>
       <c r="B45" s="19"/>
       <c r="C45" s="19"/>
       <c r="D45" s="19"/>
-      <c r="E45" s="16" t="s">
-        <v>52</v>
+      <c r="E45" s="14" t="s">
+        <v>63</v>
       </c>
       <c r="F45" s="4"/>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="15"/>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A46" s="21"/>
       <c r="B46" s="19"/>
       <c r="C46" s="19"/>
       <c r="D46" s="19"/>
-      <c r="E46" s="16" t="s">
-        <v>51</v>
+      <c r="E46" s="14" t="s">
+        <v>64</v>
       </c>
       <c r="F46" s="4"/>
     </row>
-    <row r="47" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="15"/>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A47" s="21"/>
       <c r="B47" s="19"/>
       <c r="C47" s="19"/>
       <c r="D47" s="19"/>
-      <c r="E47" s="18" t="s">
-        <v>53</v>
+      <c r="E47" s="14" t="s">
+        <v>65</v>
       </c>
       <c r="F47" s="4"/>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="15"/>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A48" s="21"/>
       <c r="B48" s="19"/>
       <c r="C48" s="19"/>
       <c r="D48" s="19"/>
-      <c r="E48" s="16" t="s">
-        <v>54</v>
+      <c r="E48" s="29" t="s">
+        <v>44</v>
       </c>
       <c r="F48" s="4"/>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="15"/>
+    <row r="49" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A49" s="21"/>
       <c r="B49" s="19"/>
       <c r="C49" s="19"/>
       <c r="D49" s="19"/>
-      <c r="E49" s="16" t="s">
-        <v>55</v>
+      <c r="E49" s="30" t="s">
+        <v>45</v>
       </c>
       <c r="F49" s="4"/>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="15"/>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A50" s="21"/>
       <c r="B50" s="19"/>
       <c r="C50" s="19"/>
       <c r="D50" s="19"/>
-      <c r="E50" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="F50" s="4"/>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="6"/>
-      <c r="B51" s="6"/>
-      <c r="C51" s="6"/>
-      <c r="D51" s="6"/>
-      <c r="E51" s="8"/>
-      <c r="F51" s="8"/>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="15">
+      <c r="E50" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="F50" s="31"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A51" s="21"/>
+      <c r="B51" s="19"/>
+      <c r="C51" s="19"/>
+      <c r="D51" s="19"/>
+      <c r="E51" s="29" t="s">
+        <v>47</v>
+      </c>
+      <c r="F51" s="31"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A52" s="21"/>
+      <c r="B52" s="19"/>
+      <c r="C52" s="19"/>
+      <c r="D52" s="19"/>
+      <c r="E52" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="F52" s="4"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A53" s="6"/>
+      <c r="B53" s="6"/>
+      <c r="C53" s="6"/>
+      <c r="D53" s="6"/>
+      <c r="E53" s="8"/>
+      <c r="F53" s="8"/>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A54" s="21">
         <v>7</v>
       </c>
-      <c r="B52" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="C52" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="D52" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="E52" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="F52" s="4"/>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="15"/>
-      <c r="B53" s="19"/>
-      <c r="C53" s="19"/>
-      <c r="D53" s="19"/>
-      <c r="E53" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="F53" s="4"/>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="15"/>
-      <c r="B54" s="19"/>
-      <c r="C54" s="19"/>
-      <c r="D54" s="19"/>
+      <c r="B54" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="C54" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="D54" s="19" t="s">
+        <v>9</v>
+      </c>
       <c r="E54" s="11" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="F54" s="4"/>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="15"/>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A55" s="21"/>
       <c r="B55" s="19"/>
       <c r="C55" s="19"/>
       <c r="D55" s="19"/>
-      <c r="E55" s="16" t="s">
-        <v>59</v>
+      <c r="E55" s="14" t="s">
+        <v>63</v>
       </c>
       <c r="F55" s="4"/>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="15"/>
+    <row r="56" spans="1:6" s="35" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A56" s="21"/>
       <c r="B56" s="19"/>
       <c r="C56" s="19"/>
       <c r="D56" s="19"/>
-      <c r="E56" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="F56" s="4"/>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="15"/>
+      <c r="E56" s="24" t="s">
+        <v>66</v>
+      </c>
+      <c r="F56" s="34"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A57" s="21"/>
       <c r="B57" s="19"/>
       <c r="C57" s="19"/>
       <c r="D57" s="19"/>
-      <c r="E57" s="16" t="s">
-        <v>60</v>
+      <c r="E57" s="11" t="s">
+        <v>67</v>
       </c>
       <c r="F57" s="4"/>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="15"/>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A58" s="21"/>
       <c r="B58" s="19"/>
       <c r="C58" s="19"/>
       <c r="D58" s="19"/>
-      <c r="E58" s="11" t="s">
-        <v>32</v>
+      <c r="E58" s="14" t="s">
+        <v>48</v>
       </c>
       <c r="F58" s="4"/>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="6"/>
-      <c r="B59" s="10"/>
-      <c r="C59" s="10"/>
-      <c r="D59" s="10"/>
-      <c r="E59" s="8"/>
-      <c r="F59" s="8"/>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="15">
-        <v>8</v>
-      </c>
-      <c r="B60" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="C60" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="D60" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="E60" s="11" t="s">
-        <v>6</v>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A59" s="21"/>
+      <c r="B59" s="19"/>
+      <c r="C59" s="19"/>
+      <c r="D59" s="19"/>
+      <c r="E59" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="F59" s="4"/>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A60" s="21"/>
+      <c r="B60" s="19"/>
+      <c r="C60" s="19"/>
+      <c r="D60" s="19"/>
+      <c r="E60" s="14" t="s">
+        <v>68</v>
       </c>
       <c r="F60" s="4"/>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="15"/>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A61" s="21"/>
       <c r="B61" s="19"/>
       <c r="C61" s="19"/>
       <c r="D61" s="19"/>
-      <c r="E61" s="16" t="s">
-        <v>56</v>
+      <c r="E61" s="14" t="s">
+        <v>49</v>
       </c>
       <c r="F61" s="4"/>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="15"/>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A62" s="21"/>
       <c r="B62" s="19"/>
       <c r="C62" s="19"/>
       <c r="D62" s="19"/>
-      <c r="E62" s="22" t="s">
-        <v>62</v>
+      <c r="E62" s="11" t="s">
+        <v>29</v>
       </c>
       <c r="F62" s="4"/>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="15"/>
-      <c r="B63" s="19"/>
-      <c r="C63" s="19"/>
-      <c r="D63" s="19"/>
-      <c r="E63" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="F63" s="4"/>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" s="6"/>
-      <c r="B64" s="10"/>
-      <c r="C64" s="10"/>
-      <c r="D64" s="10"/>
-      <c r="E64" s="8"/>
-      <c r="F64" s="8"/>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A63" s="6"/>
+      <c r="B63" s="10"/>
+      <c r="C63" s="10"/>
+      <c r="D63" s="10"/>
+      <c r="E63" s="8"/>
+      <c r="F63" s="8"/>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A64" s="21">
+        <v>8</v>
+      </c>
+      <c r="B64" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="C64" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="D64" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="E64" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="F64" s="4"/>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A65" s="21"/>
+      <c r="B65" s="19"/>
+      <c r="C65" s="19"/>
+      <c r="D65" s="19"/>
+      <c r="E65" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="F65" s="4"/>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A66" s="21"/>
+      <c r="B66" s="19"/>
+      <c r="C66" s="19"/>
+      <c r="D66" s="19"/>
+      <c r="E66" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="F66" s="4"/>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A67" s="21"/>
+      <c r="B67" s="19"/>
+      <c r="C67" s="19"/>
+      <c r="D67" s="19"/>
+      <c r="E67" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="F67" s="4"/>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A68" s="6"/>
+      <c r="B68" s="10"/>
+      <c r="C68" s="10"/>
+      <c r="D68" s="10"/>
+      <c r="E68" s="8"/>
+      <c r="F68" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="A60:A63"/>
-    <mergeCell ref="B60:B63"/>
-    <mergeCell ref="C60:C63"/>
-    <mergeCell ref="D60:D63"/>
-    <mergeCell ref="A52:A58"/>
-    <mergeCell ref="A42:A50"/>
-    <mergeCell ref="C52:C58"/>
-    <mergeCell ref="D52:D58"/>
-    <mergeCell ref="A34:A40"/>
-    <mergeCell ref="B34:B40"/>
-    <mergeCell ref="C34:C40"/>
-    <mergeCell ref="D34:D40"/>
-    <mergeCell ref="F39:F40"/>
-    <mergeCell ref="C23:C27"/>
-    <mergeCell ref="B23:B27"/>
-    <mergeCell ref="A23:A27"/>
-    <mergeCell ref="D23:D27"/>
-    <mergeCell ref="A29:A32"/>
-    <mergeCell ref="B29:B32"/>
-    <mergeCell ref="C29:C32"/>
-    <mergeCell ref="D29:D32"/>
+    <mergeCell ref="A64:A67"/>
+    <mergeCell ref="B64:B67"/>
+    <mergeCell ref="C64:C67"/>
+    <mergeCell ref="D64:D67"/>
+    <mergeCell ref="A54:A62"/>
+    <mergeCell ref="A44:A52"/>
+    <mergeCell ref="C54:C62"/>
+    <mergeCell ref="D54:D62"/>
+    <mergeCell ref="A36:A42"/>
+    <mergeCell ref="B36:B42"/>
+    <mergeCell ref="C36:C42"/>
+    <mergeCell ref="D36:D42"/>
+    <mergeCell ref="C44:C52"/>
+    <mergeCell ref="D44:D52"/>
+    <mergeCell ref="B44:B52"/>
+    <mergeCell ref="B54:B62"/>
+    <mergeCell ref="C23:C29"/>
+    <mergeCell ref="B23:B29"/>
+    <mergeCell ref="A23:A29"/>
+    <mergeCell ref="D23:D29"/>
+    <mergeCell ref="A31:A34"/>
+    <mergeCell ref="B31:B34"/>
+    <mergeCell ref="C31:C34"/>
+    <mergeCell ref="D31:D34"/>
+    <mergeCell ref="F36:F39"/>
     <mergeCell ref="A2:A11"/>
     <mergeCell ref="D13:D21"/>
     <mergeCell ref="C13:C21"/>
@@ -1490,10 +1855,6 @@
     <mergeCell ref="D2:D11"/>
     <mergeCell ref="C2:C11"/>
     <mergeCell ref="B2:B11"/>
-    <mergeCell ref="C42:C50"/>
-    <mergeCell ref="D42:D50"/>
-    <mergeCell ref="B42:B50"/>
-    <mergeCell ref="B52:B58"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>